<commit_message>
edit grafana dashboard query to get correctly filled rate + new nifi design
</commit_message>
<xml_diff>
--- a/nifi/application/config/xlsx_config/VO_UK_CONFIG.xlsx
+++ b/nifi/application/config/xlsx_config/VO_UK_CONFIG.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="VO_UK" sheetId="1" state="visible" r:id="rId2"/>
@@ -200,7 +200,7 @@
     <t xml:space="preserve">expect_column_values_to_be_phone_number</t>
   </si>
   <si>
-    <t xml:space="preserve">{'country': 'UK', 'mostly': 0.9}</t>
+    <t xml:space="preserve">{'country': 'GB', 'mostly': 0.9}</t>
   </si>
   <si>
     <t xml:space="preserve">TYPE</t>
@@ -459,8 +459,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C74" activeCellId="0" sqref="C74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1581,8 +1581,8 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>